<commit_message>
19.03 pilot gc and starting code
</commit_message>
<xml_diff>
--- a/experimental-setup/12.03 strains-for-growth-curves.xlsx
+++ b/experimental-setup/12.03 strains-for-growth-curves.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\64204\Desktop\master\experimental-setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBBEC8E-099B-4F58-A019-71CF5F3387DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437B5B77-00C9-4FD6-9289-D3A97FB70109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,7 +526,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>